<commit_message>
commit local e salvar modelo
</commit_message>
<xml_diff>
--- a/Rede Neural Inception/Resultados.xlsx
+++ b/Rede Neural Inception/Resultados.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\labin\OneDrive\Documentos\GitHub\DetectBoat-IA\Rede Neural Inception\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fb64aeaffe12d0db/Documentos/GitHub/DetectBoat-IA/Rede Neural Inception/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F24245E-9691-48D6-94A8-9C9315D33D40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="127" documentId="13_ncr:1_{3F24245E-9691-48D6-94A8-9C9315D33D40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{72288694-6393-44F3-B786-49FB932DDF2B}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20280" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
   <si>
     <t>A rede acertou 15.9% para 1 ÉPOCAS</t>
   </si>
@@ -94,12 +94,21 @@
   </si>
   <si>
     <t>Épocas: 10 | accuracy: 100.%</t>
+  </si>
+  <si>
+    <t>multicamada</t>
+  </si>
+  <si>
+    <t>epocas</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -129,8 +138,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -146,6 +159,1136 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>multicamada</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Plan1!$C$2:$C$9</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Plan1!$D$2:$D$9</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.159</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.253</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.26600000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.66600000000000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.98599999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.98599999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-A65A-47D2-82CA-25AE8D34AF1B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Convolucional</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Plan1!$C$2:$C$9</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Plan1!$E$2:$E$9</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.159</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.879</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.98599999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.98599999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-A65A-47D2-82CA-25AE8D34AF1B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Inception</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Plan1!$C$2:$C$9</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Plan1!$F$2:$F$9</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.61299999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.94599999999999995</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-A65A-47D2-82CA-25AE8D34AF1B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="537159824"/>
+        <c:axId val="537158384"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="537159824"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="537158384"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="537158384"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="537159824"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>152399</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Gráfico 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7A73FBAD-8F56-B0E5-640B-70380E0869F4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A9F0493B-A7C2-4ED9-9E28-A1010A1885D8}" name="Tabela1" displayName="Tabela1" ref="C1:F1048576" totalsRowShown="0">
+  <autoFilter ref="C1:F1048576" xr:uid="{A9F0493B-A7C2-4ED9-9E28-A1010A1885D8}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{E74B0EA4-1EA3-4BF9-BBBD-250624499A32}" name="epocas"/>
+    <tableColumn id="2" xr3:uid="{5E65071B-D89D-4BC7-9A6F-ED6FC6F642F5}" name="multicamada"/>
+    <tableColumn id="3" xr3:uid="{87687AB7-A5B5-4CE0-BD0A-2E88A4727776}" name="Convolucional"/>
+    <tableColumn id="4" xr3:uid="{19894EE3-AF44-4F1B-85B1-1FBDC40E650F}" name="Inception"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -411,88 +1554,200 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A29"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="37.42578125" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0.159</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0.159</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0.61299999999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C3" s="2">
+        <v>5</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0.253</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0.879</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0.94599999999999995</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C4" s="2">
+        <v>10</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0.26600000000000001</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0.98599999999999999</v>
+      </c>
+      <c r="F4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C5" s="2">
+        <v>30</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0.66600000000000004</v>
+      </c>
+      <c r="E5" s="1">
+        <v>1</v>
+      </c>
+      <c r="F5" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C6" s="2">
+        <v>60</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0.98599999999999999</v>
+      </c>
+      <c r="F6" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C7" s="2">
+        <v>100</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1">
+        <v>1</v>
+      </c>
+      <c r="F7" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C8" s="2">
+        <v>240</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0.98599999999999999</v>
+      </c>
+      <c r="E8" s="1">
+        <v>1</v>
+      </c>
+      <c r="F8" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C9" s="2">
+        <v>500</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0.98599999999999999</v>
+      </c>
+      <c r="E9" s="1">
+        <v>1</v>
+      </c>
+      <c r="F9" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -559,5 +1814,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>